<commit_message>
cleared output files, edited batchfile
</commit_message>
<xml_diff>
--- a/mu.xlsx
+++ b/mu.xlsx
@@ -15,80 +15,67 @@
     <sheet name="mu" sheetId="1" r:id="rId1"/>
     <sheet name="results" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Morphological Units</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>chute</t>
+  </si>
+  <si>
+    <t>fast glide</t>
+  </si>
+  <si>
+    <t>pool</t>
+  </si>
+  <si>
+    <t>riffle</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>riffle transition</t>
+  </si>
+  <si>
+    <t>slow glide</t>
+  </si>
+  <si>
+    <t>slackwater</t>
+  </si>
+  <si>
     <t>Thresholds</t>
   </si>
   <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
     <t>depth (m)</t>
   </si>
   <si>
     <t>velocity (m/s)</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>lower</t>
-  </si>
-  <si>
-    <t>upper</t>
-  </si>
-  <si>
-    <t>chute</t>
-  </si>
-  <si>
-    <t>inf</t>
-  </si>
-  <si>
-    <t>fast glide</t>
-  </si>
-  <si>
-    <t>pool</t>
-  </si>
-  <si>
-    <t>riffle</t>
-  </si>
-  <si>
-    <t>riffle transition</t>
-  </si>
-  <si>
-    <t>run</t>
-  </si>
-  <si>
-    <t>slackwater</t>
-  </si>
-  <si>
-    <t>slow glide</t>
-  </si>
-  <si>
     <t>Area (ft²) for every discharge</t>
-  </si>
-  <si>
-    <t>21100</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>880</t>
-  </si>
-  <si>
-    <t>42200</t>
-  </si>
-  <si>
-    <t>84400</t>
   </si>
 </sst>
 </file>
@@ -137,7 +124,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -189,6 +176,51 @@
         <color theme="2" tint="-9.9948118533890809E-2"/>
       </left>
       <right style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -271,6 +303,21 @@
       </right>
       <top style="thin">
         <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
       </top>
       <bottom style="thin">
         <color theme="2" tint="-9.9948118533890809E-2"/>
@@ -367,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -379,64 +426,73 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -727,77 +783,76 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="6" width="9.140625" style="2"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="27"/>
+      <c r="C3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="21"/>
-      <c r="C3" s="20" t="s">
+      <c r="C4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
         <v>2</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
-        <v>7</v>
       </c>
       <c r="C5" s="3">
         <v>0.7</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>8</v>
+      <c r="D5" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="E5" s="3">
         <v>0.9</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>9</v>
+      <c r="B6" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C6" s="4">
         <v>0.7</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="18">
         <v>1.4</v>
       </c>
       <c r="E6" s="4">
@@ -808,14 +863,14 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
-        <v>10</v>
+      <c r="B7" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="C7" s="3">
         <v>1.4</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>8</v>
+      <c r="D7" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -825,30 +880,30 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
-        <v>11</v>
+      <c r="B8" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="18">
         <v>0.7</v>
       </c>
       <c r="E8" s="4">
         <v>0.6</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
-        <v>12</v>
+      <c r="B9" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="17">
         <v>0.7</v>
       </c>
       <c r="E9" s="3">
@@ -859,14 +914,14 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>13</v>
+      <c r="B10" s="14" t="s">
+        <v>6</v>
       </c>
       <c r="C10" s="4">
         <v>0.7</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>8</v>
+      <c r="D10" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="E10" s="4">
         <v>0.6</v>
@@ -876,13 +931,13 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
-        <v>14</v>
+      <c r="B11" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="17">
         <v>1.4</v>
       </c>
       <c r="E11" s="3">
@@ -893,13 +948,13 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>15</v>
+      <c r="B12" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="19">
         <v>1.4</v>
       </c>
       <c r="E12" s="8">
@@ -917,7 +972,7 @@
     <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -931,243 +986,129 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="8" width="9.140625" style="2"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
-        <v>3168855</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1029969</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1741725</v>
-      </c>
-      <c r="F4" s="3">
-        <v>982026</v>
-      </c>
-      <c r="G4" s="3">
-        <v>4751955</v>
-      </c>
-      <c r="H4" s="6">
-        <v>6090174</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4">
-        <v>20169</v>
-      </c>
-      <c r="D5" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E5" s="4">
-        <v>11511</v>
-      </c>
-      <c r="F5" s="4">
-        <v>8937</v>
-      </c>
-      <c r="G5" s="4">
-        <v>11979</v>
-      </c>
-      <c r="H5" s="7">
-        <v>20736</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3">
-        <v>421452</v>
-      </c>
-      <c r="D6" s="3">
-        <v>30132</v>
-      </c>
-      <c r="E6" s="3">
-        <v>29475</v>
-      </c>
-      <c r="F6" s="3">
-        <v>33876</v>
-      </c>
-      <c r="G6" s="3">
-        <v>646389</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1188864</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4">
-        <v>119295</v>
-      </c>
-      <c r="D7" s="4">
-        <v>93186</v>
-      </c>
-      <c r="E7" s="4">
-        <v>92736</v>
-      </c>
-      <c r="F7" s="4">
-        <v>97659</v>
-      </c>
-      <c r="G7" s="4">
-        <v>100530</v>
-      </c>
-      <c r="H7" s="7">
-        <v>112185</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4">
-        <v>94095</v>
-      </c>
-      <c r="D9" s="4">
-        <v>57348</v>
-      </c>
-      <c r="E9" s="4">
-        <v>36693</v>
-      </c>
-      <c r="F9" s="4">
-        <v>68859</v>
-      </c>
-      <c r="G9" s="4">
-        <v>106821</v>
-      </c>
-      <c r="H9" s="7">
-        <v>310311</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="3">
-        <v>164286</v>
-      </c>
-      <c r="D10" s="3">
-        <v>46305</v>
-      </c>
-      <c r="E10" s="3">
-        <v>55152</v>
-      </c>
-      <c r="F10" s="3">
-        <v>39942</v>
-      </c>
-      <c r="G10" s="3">
-        <v>147429</v>
-      </c>
-      <c r="H10" s="6">
-        <v>164376</v>
-      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="8">
-        <v>54603</v>
-      </c>
-      <c r="D11" s="8">
-        <v>29403</v>
-      </c>
-      <c r="E11" s="8">
-        <v>29430</v>
-      </c>
-      <c r="F11" s="8">
-        <v>27864</v>
-      </c>
-      <c r="G11" s="8">
-        <v>28926</v>
-      </c>
-      <c r="H11" s="9">
-        <v>45216</v>
-      </c>
+      <c r="B11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed error: converted m to ft
</commit_message>
<xml_diff>
--- a/mu.xlsx
+++ b/mu.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klarrieu\Desktop\HYD298_02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Course\assignment_solutions\assignment_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="9645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mu" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Morphological Units</t>
   </si>
@@ -981,7 +981,7 @@
   <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1017,9 +1017,7 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="13" t="s">
-        <v>2</v>
-      </c>
+      <c r="B4" s="13"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1028,9 +1026,7 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
-        <v>3</v>
-      </c>
+      <c r="B5" s="14"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -1039,9 +1035,7 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>4</v>
-      </c>
+      <c r="B6" s="13"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1050,9 +1044,7 @@
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="B7" s="14"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1061,9 +1053,7 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="B8" s="13"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1072,9 +1062,7 @@
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>6</v>
-      </c>
+      <c r="B9" s="14"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1083,9 +1071,7 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>9</v>
-      </c>
+      <c r="B10" s="13"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1094,9 +1080,7 @@
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
-        <v>8</v>
-      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>

</xml_diff>